<commit_message>
create particiupant dans spreadshit jc
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,9 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
     <t>jc !</t>
+  </si>
+  <si>
+    <t>Simple Text</t>
+  </si>
+  <si>
+    <t>This is PhpSpreadSheet</t>
   </si>
 </sst>
 </file>
@@ -31,9 +37,9 @@
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Bahnschrift"/>
     </font>
   </fonts>
   <fills count="2">
@@ -356,7 +362,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -364,9 +370,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
php spreadsheet generate excel ok
</commit_message>
<xml_diff>
--- a/hello world.xlsx
+++ b/hello world.xlsx
@@ -15,15 +15,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>jc !</t>
-  </si>
-  <si>
-    <t>Simple Text</t>
-  </si>
-  <si>
-    <t>This is PhpSpreadSheet</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+  <si>
+    <t>Génique</t>
+  </si>
+  <si>
+    <t>Yoann</t>
+  </si>
+  <si>
+    <t>09/01/1996</t>
+  </si>
+  <si>
+    <t>genique.yoann@outlook.com</t>
+  </si>
+  <si>
+    <t>Mairot</t>
+  </si>
+  <si>
+    <t>Jean-christophe</t>
+  </si>
+  <si>
+    <t>15/05/1999</t>
+  </si>
+  <si>
+    <t>mairot.jean-christophe@gmail.com</t>
+  </si>
+  <si>
+    <t>Cherief</t>
+  </si>
+  <si>
+    <t>Saufiane</t>
+  </si>
+  <si>
+    <t>25/08/1992</t>
+  </si>
+  <si>
+    <t>saufiane.cherief@gmail.com</t>
+  </si>
+  <si>
+    <t>Rameau</t>
+  </si>
+  <si>
+    <t>Célia</t>
+  </si>
+  <si>
+    <t>13/04/2000</t>
+  </si>
+  <si>
+    <t>celia.rameau@gmail.com</t>
+  </si>
+  <si>
+    <t>Ligourel</t>
+  </si>
+  <si>
+    <t>Teedji</t>
+  </si>
+  <si>
+    <t>15/02/1997</t>
+  </si>
+  <si>
+    <t>ligourel.teedji@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -362,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -370,15 +421,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>